<commit_message>
Added new filters. Added new fields for importing, removed stale ones. Fixed importing logic. Changes on mandatory data. Added excel examples.
</commit_message>
<xml_diff>
--- a/ZZ - Documents/ImprotacionClientes.xlsx
+++ b/ZZ - Documents/ImprotacionClientes.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="T:\Carma\ZZ - Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\DiscoT\Carma\ZZ - Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3F83BB45-68FD-41F1-A7F4-4BF8368D0E48}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AB29E6BB-7128-47C4-BE5C-CC8C9300D20E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
   <si>
     <t>R. Social</t>
   </si>
@@ -31,9 +31,6 @@
     <t>Direccion</t>
   </si>
   <si>
-    <t>localidad</t>
-  </si>
-  <si>
     <t>Altura</t>
   </si>
   <si>
@@ -58,22 +55,37 @@
     <t>mengano@gmail.com</t>
   </si>
   <si>
-    <t>Cod Localidad</t>
-  </si>
-  <si>
-    <t>sociedad anonima prueba 2435</t>
-  </si>
-  <si>
-    <t>hoteles playa  b345</t>
-  </si>
-  <si>
-    <t>una clinic2 345</t>
-  </si>
-  <si>
-    <t>B1619AAA</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ESCOBAR                                                     </t>
+    <t>Nombre</t>
+  </si>
+  <si>
+    <t>Apellido</t>
+  </si>
+  <si>
+    <t>Cosme</t>
+  </si>
+  <si>
+    <t>Fulanito</t>
+  </si>
+  <si>
+    <t>Av rivadavia</t>
+  </si>
+  <si>
+    <t>Homero</t>
+  </si>
+  <si>
+    <t>Thompson</t>
+  </si>
+  <si>
+    <t>Libertad</t>
+  </si>
+  <si>
+    <t>sociedad anonima prueba 66</t>
+  </si>
+  <si>
+    <t>hoteles playa 34</t>
+  </si>
+  <si>
+    <t>una clinic2 22</t>
   </si>
 </sst>
 </file>
@@ -460,17 +472,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G4"/>
+  <dimension ref="A1:G6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J9" sqref="J9"/>
+      <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="39.85546875" customWidth="1"/>
-    <col min="2" max="2" width="12" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="23.5703125" customWidth="1"/>
+    <col min="4" max="4" width="16.85546875" customWidth="1"/>
+    <col min="5" max="5" width="20.7109375" customWidth="1"/>
+    <col min="7" max="7" width="30.85546875" customWidth="1"/>
+    <col min="13" max="13" width="23.5703125" customWidth="1"/>
+    <col min="14" max="14" width="14.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
@@ -478,98 +493,114 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="E1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="F1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" t="s">
-        <v>8</v>
-      </c>
       <c r="G1" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>13</v>
-      </c>
-      <c r="B2">
-        <v>4124564123</v>
-      </c>
-      <c r="C2" t="s">
-        <v>7</v>
-      </c>
-      <c r="D2" t="s">
-        <v>17</v>
-      </c>
-      <c r="E2">
+        <v>19</v>
+      </c>
+      <c r="D2">
+        <v>41245641235</v>
+      </c>
+      <c r="E2" t="s">
+        <v>6</v>
+      </c>
+      <c r="F2">
         <v>1235</v>
       </c>
-      <c r="F2" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="G2" t="s">
-        <v>16</v>
+      <c r="G2" s="1" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>14</v>
-      </c>
-      <c r="B3">
-        <v>7568679111</v>
-      </c>
-      <c r="C3" t="s">
-        <v>6</v>
-      </c>
-      <c r="D3" t="s">
-        <v>17</v>
-      </c>
-      <c r="E3">
+        <v>20</v>
+      </c>
+      <c r="D3">
+        <v>75686791112</v>
+      </c>
+      <c r="E3" t="s">
+        <v>5</v>
+      </c>
+      <c r="F3">
         <v>645476</v>
       </c>
-      <c r="F3" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="G3" t="s">
-        <v>16</v>
+      <c r="G3" s="1" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
+        <v>21</v>
+      </c>
+      <c r="D4">
+        <v>67698809</v>
+      </c>
+      <c r="E4" t="s">
+        <v>4</v>
+      </c>
+      <c r="F4">
+        <v>132124</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B5" t="s">
+        <v>13</v>
+      </c>
+      <c r="C5" t="s">
+        <v>14</v>
+      </c>
+      <c r="D5">
+        <v>45879855487</v>
+      </c>
+      <c r="E5" t="s">
         <v>15</v>
       </c>
-      <c r="B4">
-        <v>6769880</v>
-      </c>
-      <c r="C4" t="s">
-        <v>5</v>
-      </c>
-      <c r="D4" t="s">
+      <c r="F5">
+        <v>1245</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B6" t="s">
+        <v>16</v>
+      </c>
+      <c r="C6" t="s">
         <v>17</v>
       </c>
-      <c r="E4">
-        <v>132124</v>
-      </c>
-      <c r="F4" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="G4" t="s">
-        <v>16</v>
+      <c r="D6">
+        <v>788445145696</v>
+      </c>
+      <c r="E6" t="s">
+        <v>18</v>
+      </c>
+      <c r="F6">
+        <v>4500</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="F2" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
-    <hyperlink ref="F3" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
-    <hyperlink ref="F4" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
+    <hyperlink ref="G2" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="G3" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
+    <hyperlink ref="G4" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>